<commit_message>
class 27 Excel File reading
</commit_message>
<xml_diff>
--- a/Files/Employees.xlsx
+++ b/Files/Employees.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>FirstName</t>
   </si>
@@ -65,6 +65,15 @@
   </si>
   <si>
     <t>Tiger</t>
+  </si>
+  <si>
+    <t>Moncef</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Belgas</t>
   </si>
 </sst>
 </file>
@@ -72,10 +81,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -1003,7 +1012,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
@@ -1011,94 +1020,105 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="17.7904761904762" customWidth="1"/>
-    <col min="2" max="2" width="15.7142857142857" customWidth="1"/>
-    <col min="3" max="3" width="14.9904761904762" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.7904761904762"/>
+    <col min="2" max="2" customWidth="true" width="15.7142857142857"/>
+    <col min="3" max="3" customWidth="true" width="14.9904761904762"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>19</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0">
         <v>1250000</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <v>21</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0">
         <v>129000</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0">
         <v>200</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0">
         <v>300000</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="0">
         <v>30</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0">
         <v>90000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>